<commit_message>
add draw bar funcation
</commit_message>
<xml_diff>
--- a/output/example.xlsx
+++ b/output/example.xlsx
@@ -73,12 +73,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -87,6 +90,170 @@
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Bar Chart</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'sheet-1'!A3</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'sheet-1'!$A$3:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'sheet-1'!$A$4:$A$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'sheet-1'!B3</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'sheet-1'!$A$3:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'sheet-1'!$B$4:$B$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Sample length (mm)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>number</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,6 +595,9 @@
           <t>row-1</t>
         </is>
       </c>
+      <c r="B3" s="3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -435,6 +605,9 @@
           <t>row-2</t>
         </is>
       </c>
+      <c r="B4" s="3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -442,12 +615,18 @@
           <t>row-3</t>
         </is>
       </c>
+      <c r="B5" s="3" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
           <t>row-4</t>
         </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -455,6 +634,7 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -464,82 +644,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="1" max="2" min="2" width="20"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="15"/>
-    <col customWidth="1" max="5" min="5" width="15"/>
-    <col customWidth="1" max="6" min="6" width="15"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Examplesheet-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>col-1</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>col-2</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>col-3</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>col-4</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>row-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>row-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>row-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>row-4</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
@@ -550,82 +662,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="1" max="2" min="2" width="20"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="15"/>
-    <col customWidth="1" max="5" min="5" width="15"/>
-    <col customWidth="1" max="6" min="6" width="15"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Examplesheet-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>col-1</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>col-2</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>col-3</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>col-4</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>row-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>row-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>row-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>row-4</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>